<commit_message>
Configure authorization. Fixed bugs of Feedback. Refactoring code in Views.
</commit_message>
<xml_diff>
--- a/BlackStorkApp/Content/documents/Catalog.xlsx
+++ b/BlackStorkApp/Content/documents/Catalog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -38,24 +38,18 @@
     <t>Шлейка x-back</t>
   </si>
   <si>
-    <t>Ipsum dolor sit amet dolor sit amet dolor sit amet dolor sit amet</t>
+    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Aenean commodo ligula eget dolor. Aenean massa. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Donec quam felis, ultricies nec, pellentesque eu, pretium quis, sem. Nulla consequat massa quis enim. Donec.</t>
   </si>
   <si>
     <t>Шлейка h-back</t>
   </si>
   <si>
-    <t>Ipsum dolor sit amet</t>
-  </si>
-  <si>
     <t>Нарты спортивные</t>
   </si>
   <si>
     <t>Сумка для снаряжения</t>
   </si>
   <si>
-    <t xml:space="preserve">Ipsum dolor sit amet dolor sit amet dolor sit amet dolor sit amet dolor sit amet </t>
-  </si>
-  <si>
     <t>Дождевик</t>
   </si>
   <si>
@@ -65,7 +59,28 @@
     <t>Тапочки</t>
   </si>
   <si>
-    <t>Ipsum dolor sit amet dolor sit amet dolor sit ametdolor sit ametdolor sit ametdolor sit ametdolor sit ametdolor sit amet</t>
+    <t>Шлейка грузовая</t>
+  </si>
+  <si>
+    <t>Нарты грузовые</t>
+  </si>
+  <si>
+    <t>Сумка для формы</t>
+  </si>
+  <si>
+    <t>Дождевик в стиле БАТЭ</t>
+  </si>
+  <si>
+    <t>Бандана</t>
+  </si>
+  <si>
+    <t>Тапочки флисовые</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>relativePathrelativePath</t>
   </si>
 </sst>
 </file>
@@ -384,14 +399,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -424,7 +439,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,10 +447,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -443,10 +458,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,10 +469,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,10 +480,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -476,10 +491,98 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The update of methods for password recovery, import and export data
</commit_message>
<xml_diff>
--- a/BlackStorkApp/Content/documents/Catalog.xlsx
+++ b/BlackStorkApp/Content/documents/Catalog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -38,18 +38,24 @@
     <t>Шлейка x-back</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Aenean commodo ligula eget dolor. Aenean massa. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Donec quam felis, ultricies nec, pellentesque eu, pretium quis, sem. Nulla consequat massa quis enim. Donec.</t>
+    <t>Ipsum dolor sit amet dolor sit amet dolor sit amet dolor sit amet</t>
   </si>
   <si>
     <t>Шлейка h-back</t>
   </si>
   <si>
+    <t>Ipsum dolor sit amet</t>
+  </si>
+  <si>
     <t>Нарты спортивные</t>
   </si>
   <si>
     <t>Сумка для снаряжения</t>
   </si>
   <si>
+    <t xml:space="preserve">Ipsum dolor sit amet dolor sit amet dolor sit amet dolor sit amet dolor sit amet </t>
+  </si>
+  <si>
     <t>Дождевик</t>
   </si>
   <si>
@@ -59,28 +65,7 @@
     <t>Тапочки</t>
   </si>
   <si>
-    <t>Шлейка грузовая</t>
-  </si>
-  <si>
-    <t>Нарты грузовые</t>
-  </si>
-  <si>
-    <t>Сумка для формы</t>
-  </si>
-  <si>
-    <t>Дождевик в стиле БАТЭ</t>
-  </si>
-  <si>
-    <t>Бандана</t>
-  </si>
-  <si>
-    <t>Тапочки флисовые</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>relativePathrelativePath</t>
+    <t>Ipsum dolor sit amet dolor sit amet dolor sit ametdolor sit ametdolor sit ametdolor sit ametdolor sit ametdolor sit amet</t>
   </si>
 </sst>
 </file>
@@ -399,14 +384,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,10 +432,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,10 +443,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,10 +454,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,10 +465,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,98 +476,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
         <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>